<commit_message>
[2ª Sprint] Implementando Autenticação de usuario
</commit_message>
<xml_diff>
--- a/Backlog Projeto DSW - Helyon Pacheco.xlsx
+++ b/Backlog Projeto DSW - Helyon Pacheco.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Arquivos\IF\9º Semestre\DSW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ViagemEspacial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cenário escolhido" sheetId="1" r:id="rId1"/>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4374,8 +4374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>